<commit_message>
FEATURE: REQUERIMIENTOS Y RESPONSABILIDADES AGREGADAS PARA EL PUESTO DE ENCARGADO DE SISTEMAS
</commit_message>
<xml_diff>
--- a/descripciones/F-COS-02 Descripcion de Puestos.xlsx
+++ b/descripciones/F-COS-02 Descripcion de Puestos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosbi\Documents\documentacion_base_sistemas\descripciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9F7BEE-908D-48A4-AE16-0DC4450F6783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEB28B0-3556-4F92-9D3E-45042C97E68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
   <si>
     <t>Código</t>
   </si>
@@ -136,9 +136,6 @@
     <t>5.1</t>
   </si>
   <si>
-    <t>5.1.1</t>
-  </si>
-  <si>
     <t>5.2</t>
   </si>
   <si>
@@ -151,12 +148,6 @@
     <t>5.5</t>
   </si>
   <si>
-    <t>5.5.1</t>
-  </si>
-  <si>
-    <t>5.5.2</t>
-  </si>
-  <si>
     <t>5.6</t>
   </si>
   <si>
@@ -187,18 +178,6 @@
     <t>5.7</t>
   </si>
   <si>
-    <t>5.8</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>5.10</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
     <t>Subdirector Académico</t>
   </si>
   <si>
@@ -214,36 +193,6 @@
     <t>Dirección Académico</t>
   </si>
   <si>
-    <t>5.10.1</t>
-  </si>
-  <si>
-    <t>5.1.2</t>
-  </si>
-  <si>
-    <t>5.4.1</t>
-  </si>
-  <si>
-    <t>5.4.2</t>
-  </si>
-  <si>
-    <t>5.1.3</t>
-  </si>
-  <si>
-    <t>5.3.1</t>
-  </si>
-  <si>
-    <t>5.6.1</t>
-  </si>
-  <si>
-    <t>5.9.1</t>
-  </si>
-  <si>
-    <t>5.9.2</t>
-  </si>
-  <si>
-    <t>5.12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cobranza y vinculación académica </t>
   </si>
   <si>
@@ -289,76 +238,199 @@
     <t>F-COS-02</t>
   </si>
   <si>
+    <t>Encargado de sistemas</t>
+  </si>
+  <si>
+    <t>Direccion Academico, Direccion General</t>
+  </si>
+  <si>
+    <t>Todos los departamentos de cosbiome</t>
+  </si>
+  <si>
+    <t>Prestadores de servicios</t>
+  </si>
+  <si>
+    <t>indistinto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado Civil: </t>
+  </si>
+  <si>
+    <t>20 a 45 años</t>
+  </si>
+  <si>
+    <t>minima 1 año con lenguajes de uso "dart (flutter), javascript (reactjs, nodejs), python (tensorflow, keras) saber trabajar con metologias (scrum, canva) integradas en software jira</t>
+  </si>
+  <si>
+    <t>Programacion orientada a objetos</t>
+  </si>
+  <si>
+    <t>Patrones de diseño estandar (Singleton, Hooks, Change Notify)</t>
+  </si>
+  <si>
+    <t>MySql, NoSql</t>
+  </si>
+  <si>
+    <t>Http requets, Socket resquets</t>
+  </si>
+  <si>
+    <t>Domio de shell (zsh o sh)</t>
+  </si>
+  <si>
+    <t>Git mas a lla de git pull, push, commit, reset y add</t>
+  </si>
+  <si>
+    <t>Uso correcto de async y await para los lenjuajes javascript y dart</t>
+  </si>
+  <si>
+    <t>Null Safety para dart</t>
+  </si>
+  <si>
+    <t>Typescript sabiendo usar interfaces, types y clases</t>
+  </si>
+  <si>
+    <t>Ingles tecnico solo para documentacion de flameworks</t>
+  </si>
+  <si>
+    <t>Sitemas basados en unix para desarrollo (GNU/LINUX MacOS)</t>
+  </si>
+  <si>
+    <t>Trabajo en equipo</t>
+  </si>
+  <si>
+    <t>GitHub/GitLab para repositorios en nube</t>
+  </si>
+  <si>
+    <t>Licensiatura trunca o terminada, Bootcamps con certificacion o demostracion en prueba tecnica</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Creacion de sistemas o herramientas digitales para departamentos de empresas</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Creacion de branh o repositorio en github para el nuevo desarrollo y no comprometer viejos ya establecidos</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>Analizar requerimientos para el nuevo desarrollo y estructurar el desarrollo para codificacion</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>Codificacion de los requerimientos en servidor de pruebas implementando buenas practicas</t>
+  </si>
+  <si>
+    <t>Pruebas de desarrollo con unit testing escritos en JS y Testing Lirary</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>Presenta cambios esperar aprovacion y liberar en produccion</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Mantencion de desarrollos viejos o legacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.2.1</t>
+  </si>
+  <si>
+    <t>Buscar siempre tener actualizado desarrollo viejos con ultimas versiones de librerias o artquitecturas de diseño</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuracion de firewall de red en la oficina </t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t>Segmentar red de oficina para dispositivos conectados</t>
+  </si>
+  <si>
+    <t>4.3.2</t>
+  </si>
+  <si>
+    <t>Generar permisos de visualizacion de internet para cada dispositivo</t>
+  </si>
+  <si>
+    <t>4.3.3</t>
+  </si>
+  <si>
+    <t>Gestionar los accesos a la red interna hablando de wifi, ssh, ftp y telenet</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.4.1</t>
+  </si>
+  <si>
+    <t>Realizar conteo de los equipos de computo de la oficina</t>
+  </si>
+  <si>
+    <t>Invetarios y proteccion de equipo computacional de la oficina</t>
+  </si>
+  <si>
+    <t>4.4.2</t>
+  </si>
+  <si>
+    <t>Configuracion de bloqueos por medio de family link para radios de la empresa</t>
+  </si>
+  <si>
+    <t>Conocimiento en Testing Library (js), riverpod_testing  o Mock (Dart)</t>
+  </si>
+  <si>
+    <t>4.4.3</t>
+  </si>
+  <si>
+    <t>Configuracion de bloqueos por medio de file host en equipos de computo</t>
+  </si>
+  <si>
     <t xml:space="preserve">5. RESPONSABILIDADES , ACTIVIDADES DEL  PUESTO Y PRINCIPALES INDICADORES </t>
   </si>
   <si>
-    <t>Encargado de sistemas</t>
-  </si>
-  <si>
-    <t>Direccion Academico, Direccion General</t>
-  </si>
-  <si>
-    <t>Todos los departamentos de cosbiome</t>
-  </si>
-  <si>
-    <t>Prestadores de servicios</t>
-  </si>
-  <si>
-    <t>indistinto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado Civil: </t>
-  </si>
-  <si>
-    <t>20 a 45 años</t>
-  </si>
-  <si>
-    <t>minima 1 año con lenguajes de uso "dart (flutter), javascript (reactjs, nodejs), python (tensorflow, keras) saber trabajar con metologias (scrum, canva) integradas en software jira</t>
-  </si>
-  <si>
-    <t>Programacion orientada a objetos</t>
-  </si>
-  <si>
-    <t>Patrones de diseño estandar (Singleton, Hooks, Change Notify)</t>
-  </si>
-  <si>
-    <t>MySql, NoSql</t>
-  </si>
-  <si>
-    <t>Http requets, Socket resquets</t>
-  </si>
-  <si>
-    <t>Domio de shell (zsh o sh)</t>
-  </si>
-  <si>
-    <t>Git mas a lla de git pull, push, commit, reset y add</t>
-  </si>
-  <si>
-    <t>Uso correcto de async y await para los lenjuajes javascript y dart</t>
-  </si>
-  <si>
-    <t>Null Safety para dart</t>
-  </si>
-  <si>
-    <t>Typescript sabiendo usar interfaces, types y clases</t>
-  </si>
-  <si>
-    <t>Ingles tecnico solo para documentacion de flameworks</t>
-  </si>
-  <si>
-    <t>Sitemas basados en unix para desarrollo (GNU/LINUX MacOS)</t>
-  </si>
-  <si>
-    <t>Trabajo en equipo</t>
-  </si>
-  <si>
-    <t>GitHub/GitLab para repositorios en nube</t>
-  </si>
-  <si>
-    <t>Conocimiento de Pull Request</t>
-  </si>
-  <si>
-    <t>Licensiatura trunca o terminada, Bootcamps con certificacion o demostracion en prueba tecnica</t>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Instalacion de software requerido por departamento</t>
+  </si>
+  <si>
+    <t>4.5.1</t>
+  </si>
+  <si>
+    <t>Instalaciones de windows</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
+    <t>4.5.3</t>
+  </si>
+  <si>
+    <t>4.5.4</t>
+  </si>
+  <si>
+    <t>Instalaciones de software de terceros que se requiera para un deparmento</t>
+  </si>
+  <si>
+    <t>Instalaciones de paqueteria de office</t>
+  </si>
+  <si>
+    <t>Instalaciones de paqueteria de adobe</t>
   </si>
 </sst>
 </file>
@@ -481,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1005,6 +1077,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1013,7 +1100,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,6 +1183,249 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1114,23 +1444,11 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1141,204 +1459,6 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1387,39 +1507,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2360,23 +2483,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="59"/>
       <c r="B1" s="59"/>
       <c r="C1" s="60" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
@@ -2388,10 +2511,10 @@
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="6.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="6.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="59"/>
       <c r="C2" s="63"/>
@@ -2408,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="6.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="6.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="59"/>
       <c r="C3" s="60" t="s">
@@ -2423,7 +2546,7 @@
       <c r="J3" s="67"/>
       <c r="K3" s="69"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="63"/>
@@ -2440,7 +2563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2452,7 +2575,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>6</v>
       </c>
@@ -2467,7 +2590,7 @@
       <c r="J6" s="70"/>
       <c r="K6" s="70"/>
     </row>
-    <row r="7" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2479,60 +2602,60 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
-      <c r="D8" s="135" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="135"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
+      <c r="D8" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
-      <c r="D9" s="135" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="135"/>
-      <c r="I9" s="135"/>
-      <c r="J9" s="135"/>
-      <c r="K9" s="135"/>
-    </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
-      <c r="D10" s="135" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-    </row>
-    <row r="11" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2545,7 +2668,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
@@ -2560,7 +2683,7 @@
       <c r="J12" s="70"/>
       <c r="K12" s="70"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2572,10 +2695,10 @@
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
       <c r="K13" s="8"/>
-      <c r="M13" s="145"/>
-      <c r="N13" s="145"/>
-    </row>
-    <row r="14" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2587,10 +2710,10 @@
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
-      <c r="M14" s="145"/>
-      <c r="N14" s="145"/>
-    </row>
-    <row r="15" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2602,10 +2725,10 @@
       <c r="I15" s="3"/>
       <c r="J15" s="7"/>
       <c r="K15" s="8"/>
-      <c r="M15" s="145"/>
-      <c r="N15" s="145"/>
-    </row>
-    <row r="16" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2617,10 +2740,10 @@
       <c r="I16" s="9"/>
       <c r="J16" s="7"/>
       <c r="K16" s="8"/>
-      <c r="M16" s="145"/>
-      <c r="N16" s="145"/>
-    </row>
-    <row r="17" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2633,7 +2756,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2646,7 +2769,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="70" t="s">
         <v>11</v>
       </c>
@@ -2661,686 +2784,720 @@
       <c r="J19" s="70"/>
       <c r="K19" s="70"/>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="135" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
-      <c r="J20" s="135"/>
+      <c r="B20" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="135" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="135"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="135"/>
-      <c r="J21" s="135"/>
+      <c r="B21" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="22"/>
     </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A22" s="75" t="s">
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A22" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-    </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="139" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="139"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="54"/>
       <c r="E23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="138" t="s">
-        <v>92</v>
+      <c r="F23" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="135" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="135"/>
-    </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="140" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="58" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="58"/>
-      <c r="H24" s="141" t="s">
+      <c r="H24" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="17"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="19"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
+    </row>
+    <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="147" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="149"/>
+      <c r="D34" s="149"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
+      <c r="G34" s="149"/>
+      <c r="H34" s="149"/>
+      <c r="I34" s="149"/>
+      <c r="J34" s="149"/>
+      <c r="K34" s="150"/>
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="151" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="152"/>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="151" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="152"/>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="151" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="152"/>
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="151" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="152"/>
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="151" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="152"/>
+      <c r="O39" s="30"/>
+    </row>
+    <row r="40" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="146" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="146"/>
+      <c r="D40" s="146"/>
+      <c r="E40" s="146"/>
+      <c r="F40" s="146"/>
+      <c r="G40" s="146"/>
+      <c r="H40" s="146"/>
+      <c r="I40" s="146"/>
+      <c r="J40" s="146"/>
+      <c r="K40" s="154"/>
+      <c r="O40" s="30"/>
+    </row>
+    <row r="41" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="151" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="152"/>
+      <c r="O41" s="29"/>
+    </row>
+    <row r="42" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="153" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="146" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="146"/>
+      <c r="D42" s="146"/>
+      <c r="E42" s="146"/>
+      <c r="F42" s="146"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="146"/>
+      <c r="I42" s="146"/>
+      <c r="J42" s="146"/>
+      <c r="K42" s="154"/>
+      <c r="O42" s="29"/>
+    </row>
+    <row r="43" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="151" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="I24" s="141"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="141"/>
-    </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="136" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="136"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="136"/>
-      <c r="G25" s="136"/>
-      <c r="H25" s="136"/>
-      <c r="I25" s="136"/>
-      <c r="J25" s="136"/>
-      <c r="K25" s="136"/>
-    </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="142" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="142"/>
-      <c r="C26" s="142"/>
-      <c r="D26" s="142"/>
-      <c r="E26" s="142"/>
-      <c r="F26" s="142" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="142"/>
-      <c r="H26" s="142"/>
-      <c r="I26" s="142"/>
-      <c r="J26" s="142"/>
-      <c r="K26" s="142"/>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="141" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="141"/>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
-      <c r="E27" s="141"/>
-      <c r="F27" s="141" t="s">
-        <v>103</v>
-      </c>
-      <c r="G27" s="141"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="141"/>
-      <c r="J27" s="141"/>
-      <c r="K27" s="141"/>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="141" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="141"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="141" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="141"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
-      <c r="J29" s="141"/>
-      <c r="K29" s="141"/>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="141" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="141"/>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="141"/>
-      <c r="F30" s="141" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="141"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
-      <c r="J30" s="141"/>
-      <c r="K30" s="141"/>
-      <c r="L30" s="19"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="141" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="141"/>
-      <c r="C31" s="141"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="141"/>
-      <c r="F31" s="141" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="141"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="141"/>
-      <c r="J31" s="141"/>
-      <c r="K31" s="141"/>
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="143" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" s="143"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="144" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="144"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B33" s="133"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
-      <c r="G33" s="133"/>
-      <c r="H33" s="133"/>
-      <c r="I33" s="133"/>
-      <c r="J33" s="133"/>
-      <c r="K33" s="134"/>
-    </row>
-    <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="135"/>
-      <c r="C34" s="135"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="135"/>
-      <c r="G34" s="135"/>
-      <c r="H34" s="135"/>
-      <c r="I34" s="135"/>
-      <c r="J34" s="135"/>
-      <c r="K34" s="135"/>
-      <c r="O34" s="20"/>
-    </row>
-    <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="135"/>
-      <c r="C35" s="135"/>
-      <c r="D35" s="135"/>
-      <c r="E35" s="135"/>
-      <c r="F35" s="135"/>
-      <c r="G35" s="135"/>
-      <c r="H35" s="135"/>
-      <c r="I35" s="135"/>
-      <c r="J35" s="135"/>
-      <c r="K35" s="135"/>
-      <c r="O35" s="20"/>
-    </row>
-    <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="135"/>
-      <c r="C36" s="135"/>
-      <c r="D36" s="135"/>
-      <c r="E36" s="135"/>
-      <c r="F36" s="135"/>
-      <c r="G36" s="135"/>
-      <c r="H36" s="135"/>
-      <c r="I36" s="135"/>
-      <c r="J36" s="135"/>
-      <c r="K36" s="135"/>
-      <c r="O36" s="20"/>
-    </row>
-    <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="135"/>
-      <c r="C37" s="135"/>
-      <c r="D37" s="135"/>
-      <c r="E37" s="135"/>
-      <c r="F37" s="135"/>
-      <c r="G37" s="135"/>
-      <c r="H37" s="135"/>
-      <c r="I37" s="135"/>
-      <c r="J37" s="135"/>
-      <c r="K37" s="135"/>
-      <c r="O37" s="20"/>
-    </row>
-    <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="135"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="135"/>
-      <c r="J38" s="135"/>
-      <c r="K38" s="135"/>
-      <c r="O38" s="20"/>
-    </row>
-    <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="135"/>
-      <c r="C39" s="135"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="135"/>
-      <c r="I39" s="135"/>
-      <c r="J39" s="135"/>
-      <c r="K39" s="135"/>
-      <c r="O39" s="30"/>
-    </row>
-    <row r="40" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="135"/>
-      <c r="C40" s="135"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135"/>
-      <c r="J40" s="135"/>
-      <c r="K40" s="135"/>
-      <c r="O40" s="30"/>
-    </row>
-    <row r="41" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="135"/>
-      <c r="C41" s="135"/>
-      <c r="D41" s="135"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-      <c r="J41" s="135"/>
-      <c r="K41" s="135"/>
-      <c r="O41" s="29"/>
-    </row>
-    <row r="42" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="135"/>
-      <c r="C42" s="135"/>
-      <c r="D42" s="135"/>
-      <c r="E42" s="135"/>
-      <c r="F42" s="135"/>
-      <c r="G42" s="135"/>
-      <c r="H42" s="135"/>
-      <c r="I42" s="135"/>
-      <c r="J42" s="135"/>
-      <c r="K42" s="135"/>
-      <c r="O42" s="29"/>
-    </row>
-    <row r="43" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="135"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="135"/>
-      <c r="G43" s="135"/>
-      <c r="H43" s="135"/>
-      <c r="I43" s="135"/>
-      <c r="J43" s="135"/>
-      <c r="K43" s="135"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="152"/>
       <c r="O43" s="29"/>
     </row>
-    <row r="44" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="135"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="135"/>
-      <c r="H44" s="135"/>
-      <c r="I44" s="135"/>
-      <c r="J44" s="135"/>
-      <c r="K44" s="135"/>
+    <row r="44" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="151" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="152"/>
       <c r="O44" s="29"/>
     </row>
-    <row r="45" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="135"/>
-      <c r="C45" s="135"/>
-      <c r="D45" s="135"/>
-      <c r="E45" s="135"/>
-      <c r="F45" s="135"/>
-      <c r="G45" s="135"/>
-      <c r="H45" s="135"/>
-      <c r="I45" s="135"/>
-      <c r="J45" s="135"/>
-      <c r="K45" s="135"/>
+    <row r="45" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="151" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="152"/>
       <c r="O45" s="29"/>
     </row>
-    <row r="46" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="135"/>
-      <c r="C46" s="135"/>
-      <c r="D46" s="135"/>
-      <c r="E46" s="135"/>
-      <c r="F46" s="135"/>
-      <c r="G46" s="135"/>
-      <c r="H46" s="135"/>
-      <c r="I46" s="135"/>
-      <c r="J46" s="135"/>
-      <c r="K46" s="135"/>
+    <row r="46" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="153" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="146" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="146"/>
+      <c r="D46" s="146"/>
+      <c r="E46" s="146"/>
+      <c r="F46" s="146"/>
+      <c r="G46" s="146"/>
+      <c r="H46" s="146"/>
+      <c r="I46" s="146"/>
+      <c r="J46" s="146"/>
+      <c r="K46" s="154"/>
       <c r="O46" s="29"/>
     </row>
-    <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="135"/>
-      <c r="C47" s="135"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="135"/>
-      <c r="G47" s="135"/>
-      <c r="H47" s="135"/>
-      <c r="I47" s="135"/>
-      <c r="J47" s="135"/>
-      <c r="K47" s="135"/>
+    <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="151" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="152"/>
       <c r="O47" s="29"/>
     </row>
-    <row r="48" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="135"/>
-      <c r="C48" s="135"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="135"/>
-      <c r="F48" s="135"/>
-      <c r="G48" s="135"/>
-      <c r="H48" s="135"/>
-      <c r="I48" s="135"/>
-      <c r="J48" s="135"/>
-      <c r="K48" s="135"/>
+    <row r="48" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="151" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="152"/>
       <c r="O48" s="29"/>
     </row>
-    <row r="49" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="135"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="135"/>
-      <c r="G49" s="135"/>
-      <c r="H49" s="135"/>
-      <c r="I49" s="135"/>
-      <c r="J49" s="135"/>
-      <c r="K49" s="135"/>
+    <row r="49" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="151" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="152"/>
       <c r="O49" s="29"/>
     </row>
-    <row r="50" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="135"/>
-      <c r="C50" s="135"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="135"/>
-      <c r="F50" s="135"/>
-      <c r="G50" s="135"/>
-      <c r="H50" s="135"/>
-      <c r="I50" s="135"/>
-      <c r="J50" s="135"/>
-      <c r="K50" s="135"/>
+    <row r="50" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="153" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="146" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="146"/>
+      <c r="D50" s="146"/>
+      <c r="E50" s="146"/>
+      <c r="F50" s="146"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="146"/>
+      <c r="I50" s="146"/>
+      <c r="J50" s="146"/>
+      <c r="K50" s="154"/>
       <c r="O50" s="29"/>
     </row>
-    <row r="51" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="135"/>
-      <c r="C51" s="135"/>
-      <c r="D51" s="135"/>
-      <c r="E51" s="135"/>
-      <c r="F51" s="135"/>
-      <c r="G51" s="135"/>
-      <c r="H51" s="135"/>
-      <c r="I51" s="135"/>
-      <c r="J51" s="135"/>
-      <c r="K51" s="135"/>
+    <row r="51" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="153" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="152"/>
       <c r="O51" s="29"/>
     </row>
-    <row r="52" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" s="135"/>
-      <c r="C52" s="135"/>
-      <c r="D52" s="135"/>
-      <c r="E52" s="135"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="135"/>
-      <c r="H52" s="135"/>
-      <c r="I52" s="135"/>
-      <c r="J52" s="135"/>
-      <c r="K52" s="135"/>
+    <row r="52" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="151" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="152"/>
       <c r="O52" s="29"/>
     </row>
-    <row r="53" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="135"/>
-      <c r="C53" s="135"/>
-      <c r="D53" s="135"/>
-      <c r="E53" s="135"/>
-      <c r="F53" s="135"/>
-      <c r="G53" s="135"/>
-      <c r="H53" s="135"/>
-      <c r="I53" s="135"/>
-      <c r="J53" s="135"/>
-      <c r="K53" s="135"/>
+    <row r="53" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="151" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="152"/>
       <c r="O53" s="29"/>
     </row>
-    <row r="54" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="135"/>
-      <c r="C54" s="135"/>
-      <c r="D54" s="135"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="135"/>
-      <c r="I54" s="135"/>
-      <c r="J54" s="135"/>
-      <c r="K54" s="135"/>
+    <row r="54" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="152"/>
       <c r="O54" s="29"/>
     </row>
-    <row r="55" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="135"/>
-      <c r="C55" s="135"/>
-      <c r="D55" s="135"/>
-      <c r="E55" s="135"/>
-      <c r="F55" s="135"/>
-      <c r="G55" s="135"/>
-      <c r="H55" s="135"/>
-      <c r="I55" s="135"/>
-      <c r="J55" s="135"/>
-      <c r="K55" s="135"/>
+    <row r="55" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="151"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="152"/>
       <c r="O55" s="29"/>
     </row>
-    <row r="56" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="135"/>
-      <c r="C56" s="135"/>
-      <c r="D56" s="135"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="135"/>
-      <c r="H56" s="135"/>
-      <c r="I56" s="135"/>
-      <c r="J56" s="135"/>
-      <c r="K56" s="135"/>
+    <row r="56" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="153"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="152"/>
       <c r="O56" s="29"/>
     </row>
-    <row r="57" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="135"/>
-      <c r="C57" s="135"/>
-      <c r="D57" s="135"/>
-      <c r="E57" s="135"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="135"/>
-      <c r="H57" s="135"/>
-      <c r="I57" s="135"/>
-      <c r="J57" s="135"/>
-      <c r="K57" s="135"/>
+    <row r="57" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="151"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="152"/>
       <c r="O57" s="29"/>
     </row>
-    <row r="58" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="135"/>
-      <c r="C58" s="135"/>
-      <c r="D58" s="135"/>
-      <c r="E58" s="135"/>
-      <c r="F58" s="135"/>
-      <c r="G58" s="135"/>
-      <c r="H58" s="135"/>
-      <c r="I58" s="135"/>
-      <c r="J58" s="135"/>
-      <c r="K58" s="135"/>
+    <row r="58" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="153"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="152"/>
       <c r="O58" s="29"/>
     </row>
-    <row r="59" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
-      <c r="B59" s="135"/>
-      <c r="C59" s="135"/>
-      <c r="D59" s="135"/>
-      <c r="E59" s="135"/>
-      <c r="F59" s="135"/>
-      <c r="G59" s="135"/>
-      <c r="H59" s="135"/>
-      <c r="I59" s="135"/>
-      <c r="J59" s="135"/>
-      <c r="K59" s="135"/>
+    <row r="59" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="151"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="152"/>
       <c r="O59" s="29"/>
     </row>
-    <row r="60" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="137"/>
-      <c r="B60" s="135"/>
-      <c r="C60" s="135"/>
-      <c r="D60" s="135"/>
-      <c r="E60" s="135"/>
-      <c r="F60" s="135"/>
-      <c r="G60" s="135"/>
-      <c r="H60" s="135"/>
-      <c r="I60" s="135"/>
-      <c r="J60" s="135"/>
-      <c r="K60" s="135"/>
+    <row r="60" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="155"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="156"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="156"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="156"/>
+      <c r="H60" s="156"/>
+      <c r="I60" s="156"/>
+      <c r="J60" s="156"/>
+      <c r="K60" s="157"/>
       <c r="O60" s="29"/>
     </row>
-    <row r="61" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="25"/>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
@@ -3353,84 +3510,84 @@
       <c r="J61" s="23"/>
       <c r="K61" s="23"/>
     </row>
-    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="51" t="s">
+    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="52"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="53"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="47"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="54" t="s">
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+      <c r="J62" s="47"/>
+      <c r="K62" s="48"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="49"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D63" s="55"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="54" t="s">
+      <c r="D63" s="52"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="55"/>
-      <c r="H63" s="55"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="54" t="s">
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="K63" s="56"/>
-    </row>
-    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="54" t="s">
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B64" s="56"/>
-      <c r="C64" s="135"/>
-      <c r="D64" s="135"/>
-      <c r="E64" s="135"/>
-      <c r="F64" s="135"/>
-      <c r="G64" s="135"/>
-      <c r="H64" s="135"/>
-      <c r="I64" s="135"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="46"/>
-    </row>
-    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="54" t="s">
+      <c r="B64" s="53"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="50"/>
+    </row>
+    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="56"/>
-      <c r="C65" s="135"/>
-      <c r="D65" s="135"/>
-      <c r="E65" s="135"/>
-      <c r="F65" s="135"/>
-      <c r="G65" s="135"/>
-      <c r="H65" s="135"/>
-      <c r="I65" s="135"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="46"/>
-    </row>
-    <row r="66" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54" t="s">
+      <c r="B65" s="53"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="50"/>
+    </row>
+    <row r="66" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="56"/>
-      <c r="C66" s="135"/>
-      <c r="D66" s="135"/>
-      <c r="E66" s="135"/>
-      <c r="F66" s="135"/>
-      <c r="G66" s="135"/>
-      <c r="H66" s="135"/>
-      <c r="I66" s="135"/>
-      <c r="J66" s="47"/>
-      <c r="K66" s="46"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="84">
@@ -3534,13 +3691,13 @@
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59"/>
       <c r="B1" s="59"/>
       <c r="C1" s="60" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
@@ -3553,16 +3710,16 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="59"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
       <c r="J2" s="66" t="s">
         <v>1</v>
       </c>
@@ -3570,7 +3727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="59"/>
       <c r="C3" s="63"/>
@@ -3583,7 +3740,7 @@
       <c r="J3" s="67"/>
       <c r="K3" s="69"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="63" t="s">
@@ -3602,7 +3759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3614,7 +3771,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>6</v>
       </c>
@@ -3629,7 +3786,7 @@
       <c r="J6" s="70"/>
       <c r="K6" s="70"/>
     </row>
-    <row r="7" spans="1:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -3641,60 +3798,60 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="71" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
-      <c r="D8" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="82"/>
+      <c r="D8" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="83"/>
       <c r="K8" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
-      <c r="D9" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="84" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
-      <c r="D10" s="84" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="86"/>
-    </row>
-    <row r="11" spans="1:11" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="87"/>
+    </row>
+    <row r="11" spans="1:11" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3707,7 +3864,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
@@ -3722,7 +3879,7 @@
       <c r="J12" s="70"/>
       <c r="K12" s="70"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3735,7 +3892,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3748,7 +3905,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3761,7 +3918,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3774,7 +3931,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -3787,7 +3944,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3800,7 +3957,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>11</v>
       </c>
@@ -3815,64 +3972,64 @@
       <c r="J19" s="70"/>
       <c r="K19" s="70"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="93"/>
+      <c r="B20" s="92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="94"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="95"/>
+      <c r="B21" s="95" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="96"/>
       <c r="K21" s="22"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="96" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="96"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="97" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="97"/>
       <c r="E23" s="27" t="s">
         <v>15</v>
       </c>
@@ -3882,562 +4039,562 @@
       <c r="G23" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="96" t="s">
+      <c r="H23" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-    </row>
-    <row r="24" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="57" t="s">
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+    </row>
+    <row r="24" spans="1:11" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="97" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="98" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
       <c r="F24" s="58" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="58"/>
-      <c r="H24" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="97"/>
-      <c r="J24" s="97"/>
-      <c r="K24" s="97"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="42" t="s">
+      <c r="H24" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="98"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="87" t="s">
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="101"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="89" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="89"/>
-      <c r="H26" s="89"/>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="90"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="98" t="s">
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="91"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="100"/>
-      <c r="J27" s="100"/>
-      <c r="K27" s="101"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="102" t="s">
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="105"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="104"/>
-      <c r="K28" s="105"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="98" t="s">
+      <c r="B28" s="107"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="109"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="108"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="109" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
-      <c r="K30" s="105"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="111" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="112"/>
-      <c r="C31" s="112"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="108"/>
-    </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="41"/>
-    </row>
-    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="48" t="s">
+      <c r="B29" s="110"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="110"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="112"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="113" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="109"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="115" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="116"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="111"/>
+      <c r="H31" s="111"/>
+      <c r="I31" s="111"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="112"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="120"/>
+      <c r="C32" s="120"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="124"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="50"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="128"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="129"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="117"/>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
-      <c r="F34" s="117"/>
-      <c r="G34" s="117"/>
-      <c r="H34" s="117"/>
-      <c r="I34" s="117"/>
-      <c r="J34" s="117"/>
-      <c r="K34" s="117"/>
+      <c r="B34" s="130"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="130"/>
+      <c r="E34" s="130"/>
+      <c r="F34" s="130"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="130"/>
+      <c r="J34" s="130"/>
+      <c r="K34" s="130"/>
       <c r="L34" s="34"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="118" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="118"/>
+      <c r="B35" s="131" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="131"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="131"/>
+      <c r="F35" s="131"/>
+      <c r="G35" s="131"/>
+      <c r="H35" s="131"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="131"/>
+      <c r="K35" s="131"/>
       <c r="L35" s="34"/>
       <c r="N35" s="29"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="118" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="118"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="118"/>
-      <c r="K36" s="118"/>
+        <v>36</v>
+      </c>
+      <c r="B36" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="131"/>
+      <c r="I36" s="131"/>
+      <c r="J36" s="131"/>
+      <c r="K36" s="131"/>
       <c r="L36" s="34"/>
       <c r="N36" s="29"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="118" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="118"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="118"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="131" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="131"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="131"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="131"/>
+      <c r="K37" s="131"/>
       <c r="L37" s="34"/>
       <c r="N37" s="29"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="118" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="118"/>
+        <v>38</v>
+      </c>
+      <c r="B38" s="131" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="131"/>
+      <c r="D38" s="131"/>
+      <c r="E38" s="131"/>
+      <c r="F38" s="131"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="131"/>
+      <c r="K38" s="131"/>
       <c r="L38" s="34"/>
       <c r="N38" s="29"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="118" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="118"/>
-      <c r="J39" s="118"/>
-      <c r="K39" s="118"/>
+        <v>39</v>
+      </c>
+      <c r="B39" s="131" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="131"/>
+      <c r="D39" s="131"/>
+      <c r="E39" s="131"/>
+      <c r="F39" s="131"/>
+      <c r="G39" s="131"/>
+      <c r="H39" s="131"/>
+      <c r="I39" s="131"/>
+      <c r="J39" s="131"/>
+      <c r="K39" s="131"/>
       <c r="L39" s="34"/>
       <c r="N39" s="29"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="118" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118"/>
-      <c r="J40" s="118"/>
-      <c r="K40" s="118"/>
+        <v>40</v>
+      </c>
+      <c r="B40" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="131"/>
+      <c r="D40" s="131"/>
+      <c r="E40" s="131"/>
+      <c r="F40" s="131"/>
+      <c r="G40" s="131"/>
+      <c r="H40" s="131"/>
+      <c r="I40" s="131"/>
+      <c r="J40" s="131"/>
+      <c r="K40" s="131"/>
       <c r="L40" s="34"/>
       <c r="N40" s="29"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="118" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
-      <c r="I41" s="118"/>
-      <c r="J41" s="118"/>
-      <c r="K41" s="118"/>
+        <v>49</v>
+      </c>
+      <c r="B41" s="131" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="131"/>
+      <c r="D41" s="131"/>
+      <c r="E41" s="131"/>
+      <c r="F41" s="131"/>
+      <c r="G41" s="131"/>
+      <c r="H41" s="131"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
       <c r="L41" s="34"/>
       <c r="N41" s="29"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
-      <c r="B42" s="119"/>
-      <c r="C42" s="119"/>
-      <c r="D42" s="119"/>
-      <c r="E42" s="119"/>
-      <c r="F42" s="119"/>
-      <c r="G42" s="119"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="119"/>
-      <c r="J42" s="119"/>
-      <c r="K42" s="120"/>
+      <c r="B42" s="132"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="132"/>
+      <c r="E42" s="132"/>
+      <c r="F42" s="132"/>
+      <c r="G42" s="132"/>
+      <c r="H42" s="132"/>
+      <c r="I42" s="132"/>
+      <c r="J42" s="132"/>
+      <c r="K42" s="133"/>
       <c r="L42" s="34"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
-      <c r="B43" s="119"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="119"/>
-      <c r="G43" s="119"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="119"/>
-      <c r="J43" s="119"/>
-      <c r="K43" s="120"/>
+      <c r="B43" s="132"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="132"/>
+      <c r="E43" s="132"/>
+      <c r="F43" s="132"/>
+      <c r="G43" s="132"/>
+      <c r="H43" s="132"/>
+      <c r="I43" s="132"/>
+      <c r="J43" s="132"/>
+      <c r="K43" s="133"/>
       <c r="L43" s="34"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="33"/>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="115"/>
-      <c r="I44" s="115"/>
-      <c r="J44" s="115"/>
-      <c r="K44" s="116"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="125"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="125"/>
+      <c r="F44" s="125"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="125"/>
+      <c r="I44" s="125"/>
+      <c r="J44" s="125"/>
+      <c r="K44" s="126"/>
       <c r="L44" s="34"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
-      <c r="B45" s="120"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="120"/>
-      <c r="J45" s="120"/>
-      <c r="K45" s="120"/>
+      <c r="B45" s="133"/>
+      <c r="C45" s="133"/>
+      <c r="D45" s="133"/>
+      <c r="E45" s="133"/>
+      <c r="F45" s="133"/>
+      <c r="G45" s="133"/>
+      <c r="H45" s="133"/>
+      <c r="I45" s="133"/>
+      <c r="J45" s="133"/>
+      <c r="K45" s="133"/>
       <c r="L45" s="34"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="33"/>
-      <c r="B46" s="115"/>
-      <c r="C46" s="115"/>
-      <c r="D46" s="115"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="115"/>
-      <c r="I46" s="115"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="116"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="125"/>
+      <c r="F46" s="125"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="125"/>
+      <c r="I46" s="125"/>
+      <c r="J46" s="125"/>
+      <c r="K46" s="126"/>
       <c r="L46" s="34"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
-      <c r="B47" s="122"/>
-      <c r="C47" s="122"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="122"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="122"/>
-      <c r="K47" s="123"/>
+      <c r="B47" s="135"/>
+      <c r="C47" s="135"/>
+      <c r="D47" s="135"/>
+      <c r="E47" s="135"/>
+      <c r="F47" s="135"/>
+      <c r="G47" s="135"/>
+      <c r="H47" s="135"/>
+      <c r="I47" s="135"/>
+      <c r="J47" s="135"/>
+      <c r="K47" s="136"/>
       <c r="L47" s="34"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="33"/>
-      <c r="B48" s="115"/>
-      <c r="C48" s="115"/>
-      <c r="D48" s="115"/>
-      <c r="E48" s="115"/>
-      <c r="F48" s="115"/>
-      <c r="G48" s="115"/>
-      <c r="H48" s="115"/>
-      <c r="I48" s="115"/>
-      <c r="J48" s="115"/>
-      <c r="K48" s="116"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="125"/>
+      <c r="F48" s="125"/>
+      <c r="G48" s="125"/>
+      <c r="H48" s="125"/>
+      <c r="I48" s="125"/>
+      <c r="J48" s="125"/>
+      <c r="K48" s="126"/>
       <c r="L48" s="34"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
-      <c r="B49" s="115"/>
-      <c r="C49" s="115"/>
-      <c r="D49" s="115"/>
-      <c r="E49" s="115"/>
-      <c r="F49" s="115"/>
-      <c r="G49" s="115"/>
-      <c r="H49" s="115"/>
-      <c r="I49" s="115"/>
-      <c r="J49" s="115"/>
-      <c r="K49" s="124"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="125"/>
+      <c r="C49" s="125"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="125"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="125"/>
+      <c r="I49" s="125"/>
+      <c r="J49" s="125"/>
+      <c r="K49" s="137"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
-      <c r="B50" s="115"/>
-      <c r="C50" s="115"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="115"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="115"/>
-      <c r="I50" s="115"/>
-      <c r="J50" s="115"/>
-      <c r="K50" s="124"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="125"/>
+      <c r="F50" s="125"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="125"/>
+      <c r="I50" s="125"/>
+      <c r="J50" s="125"/>
+      <c r="K50" s="137"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="32"/>
-      <c r="B51" s="122"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
-      <c r="G51" s="122"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="122"/>
-      <c r="J51" s="122"/>
-      <c r="K51" s="125"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="135"/>
+      <c r="C51" s="135"/>
+      <c r="D51" s="135"/>
+      <c r="E51" s="135"/>
+      <c r="F51" s="135"/>
+      <c r="G51" s="135"/>
+      <c r="H51" s="135"/>
+      <c r="I51" s="135"/>
+      <c r="J51" s="135"/>
+      <c r="K51" s="138"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="32"/>
-      <c r="B52" s="122"/>
-      <c r="C52" s="122"/>
-      <c r="D52" s="122"/>
-      <c r="E52" s="122"/>
-      <c r="F52" s="122"/>
-      <c r="G52" s="122"/>
-      <c r="H52" s="122"/>
-      <c r="I52" s="122"/>
-      <c r="J52" s="122"/>
-      <c r="K52" s="125"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="135"/>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135"/>
+      <c r="E52" s="135"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
+      <c r="H52" s="135"/>
+      <c r="I52" s="135"/>
+      <c r="J52" s="135"/>
+      <c r="K52" s="138"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="33"/>
-      <c r="B53" s="115"/>
-      <c r="C53" s="115"/>
-      <c r="D53" s="115"/>
-      <c r="E53" s="115"/>
-      <c r="F53" s="115"/>
-      <c r="G53" s="115"/>
-      <c r="H53" s="115"/>
-      <c r="I53" s="115"/>
-      <c r="J53" s="115"/>
-      <c r="K53" s="124"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="125"/>
+      <c r="C53" s="125"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="125"/>
+      <c r="F53" s="125"/>
+      <c r="G53" s="125"/>
+      <c r="H53" s="125"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="125"/>
+      <c r="K53" s="137"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
-      <c r="B54" s="119"/>
-      <c r="C54" s="119"/>
-      <c r="D54" s="119"/>
-      <c r="E54" s="119"/>
-      <c r="F54" s="119"/>
-      <c r="G54" s="119"/>
-      <c r="H54" s="119"/>
-      <c r="I54" s="119"/>
-      <c r="J54" s="119"/>
-      <c r="K54" s="121"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="132"/>
+      <c r="C54" s="132"/>
+      <c r="D54" s="132"/>
+      <c r="E54" s="132"/>
+      <c r="F54" s="132"/>
+      <c r="G54" s="132"/>
+      <c r="H54" s="132"/>
+      <c r="I54" s="132"/>
+      <c r="J54" s="132"/>
+      <c r="K54" s="134"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="33"/>
-      <c r="B55" s="115"/>
-      <c r="C55" s="115"/>
-      <c r="D55" s="115"/>
-      <c r="E55" s="115"/>
-      <c r="F55" s="115"/>
-      <c r="G55" s="115"/>
-      <c r="H55" s="115"/>
-      <c r="I55" s="115"/>
-      <c r="J55" s="115"/>
-      <c r="K55" s="124"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="125"/>
+      <c r="C55" s="125"/>
+      <c r="D55" s="125"/>
+      <c r="E55" s="125"/>
+      <c r="F55" s="125"/>
+      <c r="G55" s="125"/>
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="125"/>
+      <c r="K55" s="137"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="32"/>
-      <c r="B56" s="120"/>
-      <c r="C56" s="120"/>
-      <c r="D56" s="120"/>
-      <c r="E56" s="120"/>
-      <c r="F56" s="120"/>
-      <c r="G56" s="120"/>
-      <c r="H56" s="120"/>
-      <c r="I56" s="120"/>
-      <c r="J56" s="120"/>
-      <c r="K56" s="121"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="133"/>
+      <c r="C56" s="133"/>
+      <c r="D56" s="133"/>
+      <c r="E56" s="133"/>
+      <c r="F56" s="133"/>
+      <c r="G56" s="133"/>
+      <c r="H56" s="133"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="134"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="33"/>
-      <c r="B57" s="126"/>
-      <c r="C57" s="126"/>
-      <c r="D57" s="126"/>
-      <c r="E57" s="126"/>
-      <c r="F57" s="126"/>
-      <c r="G57" s="126"/>
-      <c r="H57" s="126"/>
-      <c r="I57" s="126"/>
-      <c r="J57" s="126"/>
-      <c r="K57" s="127"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="139"/>
+      <c r="C57" s="139"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="139"/>
+      <c r="F57" s="139"/>
+      <c r="G57" s="139"/>
+      <c r="H57" s="139"/>
+      <c r="I57" s="139"/>
+      <c r="J57" s="139"/>
+      <c r="K57" s="140"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="32"/>
-      <c r="B58" s="128"/>
-      <c r="C58" s="128"/>
-      <c r="D58" s="128"/>
-      <c r="E58" s="128"/>
-      <c r="F58" s="128"/>
-      <c r="G58" s="128"/>
-      <c r="H58" s="128"/>
-      <c r="I58" s="128"/>
-      <c r="J58" s="128"/>
-      <c r="K58" s="129"/>
-    </row>
-    <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="141"/>
+      <c r="C58" s="141"/>
+      <c r="D58" s="141"/>
+      <c r="E58" s="141"/>
+      <c r="F58" s="141"/>
+      <c r="G58" s="141"/>
+      <c r="H58" s="141"/>
+      <c r="I58" s="141"/>
+      <c r="J58" s="141"/>
+      <c r="K58" s="142"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="26"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="130"/>
-      <c r="D59" s="130"/>
-      <c r="E59" s="130"/>
-      <c r="F59" s="130"/>
-      <c r="G59" s="130"/>
-      <c r="H59" s="130"/>
-      <c r="I59" s="130"/>
-      <c r="J59" s="130"/>
-      <c r="K59" s="131"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="143"/>
+      <c r="C59" s="143"/>
+      <c r="D59" s="143"/>
+      <c r="E59" s="143"/>
+      <c r="F59" s="143"/>
+      <c r="G59" s="143"/>
+      <c r="H59" s="143"/>
+      <c r="I59" s="143"/>
+      <c r="J59" s="143"/>
+      <c r="K59" s="144"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="25"/>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
@@ -4450,96 +4607,96 @@
       <c r="J60" s="23"/>
       <c r="K60" s="23"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="51" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B61" s="52"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="53"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="47"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="54" t="s">
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="48"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="49"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="55"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="54" t="s">
+      <c r="D62" s="52"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="56"/>
-      <c r="J62" s="54" t="s">
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="53"/>
+      <c r="J62" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="K62" s="56"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="54" t="s">
+      <c r="K62" s="53"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="56"/>
-      <c r="C63" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="D63" s="132"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G63" s="132"/>
-      <c r="H63" s="132"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="46"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="54" t="s">
+      <c r="B63" s="53"/>
+      <c r="C63" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="145"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" s="145"/>
+      <c r="H63" s="145"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="50"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="56"/>
-      <c r="C64" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="132"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="G64" s="132"/>
-      <c r="H64" s="132"/>
-      <c r="I64" s="46"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="46"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="54" t="s">
+      <c r="B64" s="53"/>
+      <c r="C64" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="145"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G64" s="145"/>
+      <c r="H64" s="145"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="50"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="56"/>
-      <c r="C65" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="132"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="G65" s="132"/>
-      <c r="H65" s="132"/>
-      <c r="I65" s="46"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="46"/>
+      <c r="B65" s="53"/>
+      <c r="C65" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="145"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="G65" s="145"/>
+      <c r="H65" s="145"/>
+      <c r="I65" s="50"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="83">

</xml_diff>